<commit_message>
section three plus figures
</commit_message>
<xml_diff>
--- a/Algorithm/Test results/tests-version2.xlsx
+++ b/Algorithm/Test results/tests-version2.xlsx
@@ -26,16 +26,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
   <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
     <t>Number of Services</t>
   </si>
   <si>
     <t>2-10</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>Test 2</t>
   </si>
 </sst>
 </file>
@@ -185,7 +185,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Q1</c:v>
+                  <c:v>Test 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -263,7 +263,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Q2</c:v>
+                  <c:v>Test 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -342,11 +342,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="201566080"/>
-        <c:axId val="202541952"/>
+        <c:axId val="123584208"/>
+        <c:axId val="123584768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="201566080"/>
+        <c:axId val="123584208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -445,7 +445,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202541952"/>
+        <c:crossAx val="123584768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -453,7 +453,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202541952"/>
+        <c:axId val="123584768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -560,7 +560,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201566080"/>
+        <c:crossAx val="123584208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -727,7 +727,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Q1</c:v>
+                  <c:v>Test 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -818,7 +818,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Q2</c:v>
+                  <c:v>Test 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -910,11 +910,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="201649856"/>
-        <c:axId val="201652096"/>
+        <c:axId val="122522016"/>
+        <c:axId val="184539504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="201649856"/>
+        <c:axId val="122522016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1013,7 +1013,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201652096"/>
+        <c:crossAx val="184539504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1021,7 +1021,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="201652096"/>
+        <c:axId val="184539504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1128,7 +1128,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201649856"/>
+        <c:crossAx val="122522016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2625,8 +2625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D5:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2637,13 +2637,13 @@
   <sheetData>
     <row r="5" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="4:6" x14ac:dyDescent="0.25">
@@ -2736,18 +2736,18 @@
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>0</v>

</xml_diff>